<commit_message>
Update additional country ssp file
</commit_message>
<xml_diff>
--- a/data/data_processing/additional_country_ssp_data_sources.xlsx
+++ b/data/data_processing/additional_country_ssp_data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/.julia/dev/MimiCIAM/data/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC559E6-4F43-D14F-A341-BD82C795FFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61912B6B-8730-3E4A-8B81-120C2C0D0344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16880" yWindow="500" windowWidth="24080" windowHeight="22540" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
+    <workbookView xWindow="20460" yWindow="500" windowWidth="20500" windowHeight="22540" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="6" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update all population files with new countries
</commit_message>
<xml_diff>
--- a/data/data_processing/additional_country_ssp_data_sources.xlsx
+++ b/data/data_processing/additional_country_ssp_data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/.julia/dev/MimiCIAM/data/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61912B6B-8730-3E4A-8B81-120C2C0D0344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46192696-7FCB-584A-976B-14705B71ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="500" windowWidth="20500" windowHeight="22540" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
+    <workbookView xWindow="13160" yWindow="500" windowWidth="27800" windowHeight="22540" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ypcc" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">population!$A$1:$X$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">population!$A$1:$X$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ypcc!$A$2:$X$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A8E653-697A-354B-91C0-86AB149D73BC}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2477,7 +2477,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update all ypcc values with additional countries
</commit_message>
<xml_diff>
--- a/data/data_processing/additional_country_ssp_data_sources.xlsx
+++ b/data/data_processing/additional_country_ssp_data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisarennels/.julia/dev/MimiCIAM/data/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46192696-7FCB-584A-976B-14705B71ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF684F-8D67-C24E-A58C-63197095393E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="500" windowWidth="27800" windowHeight="22540" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
+    <workbookView xWindow="20240" yWindow="500" windowWidth="20720" windowHeight="22540" activeTab="2" xr2:uid="{71E2015E-9FF5-A841-96E7-E352D418F6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="6" r:id="rId1"/>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A8E653-697A-354B-91C0-86AB149D73BC}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -4079,8 +4079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36903805-3648-8943-9A1D-099A22B3E409}">
   <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>